<commit_message>
Add Linear Interpolation methods and linear testing.
</commit_message>
<xml_diff>
--- a/Otros/exponential_test.xlsx
+++ b/Otros/exponential_test.xlsx
@@ -7,8 +7,8 @@
     <workbookView xWindow="120" yWindow="105" windowWidth="23715" windowHeight="9285"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="cubic" sheetId="1" r:id="rId1"/>
+    <sheet name="lineal" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="145621"/>
@@ -35,7 +35,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="168" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
@@ -74,7 +74,7 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -125,7 +125,7 @@
           <c:order val="0"/>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja1!$E$3:$E$9</c:f>
+              <c:f>cubic!$E$3:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -155,7 +155,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$F$3:$F$9</c:f>
+              <c:f>cubic!$F$3:$F$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -190,7 +190,7 @@
           <c:order val="1"/>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja1!$E$3:$E$9</c:f>
+              <c:f>cubic!$E$3:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -220,7 +220,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$G$3:$G$9</c:f>
+              <c:f>cubic!$G$3:$G$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -255,7 +255,7 @@
           <c:order val="2"/>
           <c:xVal>
             <c:numRef>
-              <c:f>Hoja1!$E$3:$E$9</c:f>
+              <c:f>cubic!$E$3:$E$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -285,7 +285,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Hoja1!$H$3:$H$9</c:f>
+              <c:f>cubic!$H$3:$H$9</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="7"/>
@@ -323,11 +323,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="320841600"/>
-        <c:axId val="320840064"/>
+        <c:axId val="206441088"/>
+        <c:axId val="206442880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="320841600"/>
+        <c:axId val="206441088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -337,12 +337,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="320840064"/>
+        <c:crossAx val="206442880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="320840064"/>
+        <c:axId val="206442880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -353,7 +353,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="320841600"/>
+        <c:crossAx val="206441088"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -738,7 +738,7 @@
   <dimension ref="E2:H11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -780,7 +780,7 @@
         <v>1</v>
       </c>
       <c r="F4" s="2">
-        <f t="shared" ref="F4:F11" si="0">EXP(E4)</f>
+        <f t="shared" ref="F4:F9" si="0">EXP(E4)</f>
         <v>2.7182818284590451</v>
       </c>
       <c r="G4">
@@ -881,7 +881,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:B19"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>